<commit_message>
feat: manual categorization complete - 96 articles
Categorization:
- All 96 articles manually categorized
- Categories: Alimentation, Transport, Loisirs, etc.
- Sub-categories: 2-level hierarchy
- Interactive script used for efficiency

Scripts:
- import_articles_to_db.py: Import Excel to DuckDB
- categorize_interactive.py v1.1: Interactive categorization tool

Database:
- Added columns: category_main, category_sub, tags
- All articles now have primary category
- Sub-categories assigned

Next:
- Re-export to Power BI with categories
- Update dashboard with category visuals
- Future: Smart learning categorization
</commit_message>
<xml_diff>
--- a/finance-system/exports/powerbi/transactions.xlsx
+++ b/finance-system/exports/powerbi/transactions.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L97"/>
+  <dimension ref="A1:K97"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -493,11 +493,6 @@
           <t>raw_data</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>created_at</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -543,9 +538,6 @@
           <t>{"enseigne": "E.Leclerc", "magasin": "LECLERC STATION 24/24", "date": "2025-09-23", "heure": "23:58:53", "type_transaction": "retrait", "article": "Billet banques", "quantite": "1", "unite": "unit\u00e9", "prix_unitaire": "40.00", "prix_total": "40.00", "total_ticket": "40.00", "tva_taux": "", "tva_montant": ""}</t>
         </is>
       </c>
-      <c r="L2" s="2" t="n">
-        <v>45973.95877880897</v>
-      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -591,9 +583,6 @@
           <t>{"enseigne": "TotalEnergies", "magasin": "MESSIMY", "date": "2025-10-03", "heure": "19:43:02", "article": "DIESEL pompe 02", "quantite": "10.04", "unite": "litres", "prix_unitaire": "1.706", "prix_total": "17.13", "total_ttc": "17.13", "tva_taux": "20.00", "tva_montant": "2.86", "total_ht": "14.27"}</t>
         </is>
       </c>
-      <c r="L3" s="2" t="n">
-        <v>45973.95877880897</v>
-      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -639,9 +628,6 @@
           <t>{"enseigne": "TotalEnergies", "magasin": "RELAIS FONTAINES MARRONNIERS", "date": "2025-10-04", "heure": "17:37:16", "type_transaction": "achat", "article": "DIESEL pompe 05", "quantite": "8.99", "unite": "litres", "prix_unitaire": "1.599", "prix_total": "14.38", "total_ticket": "14.38", "tva_taux": "20.00", "tva_montant": "2.40"}</t>
         </is>
       </c>
-      <c r="L4" s="2" t="n">
-        <v>45973.95877880897</v>
-      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -687,9 +673,6 @@
           <t>{"enseigne": "E.Leclerc", "magasin": "Espace Technique E.Leclerc", "date": "2025-10-07", "heure": "19:21", "article": "Console Switch 2", "prix_unitaire": "459.00", "quantite": "1", "prix_total": "459.00", "total_ticket": "524.85"}</t>
         </is>
       </c>
-      <c r="L5" s="2" t="n">
-        <v>45973.95877880897</v>
-      </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -735,9 +718,6 @@
           <t>{"enseigne": "E.Leclerc", "magasin": "Espace Technique E.Leclerc", "date": "2025-10-07", "heure": "19:21", "article": "Batterie Ecran 3D Samsung Q S24", "prix_unitaire": "15.90", "quantite": "1", "prix_total": "15.90", "total_ticket": "524.85"}</t>
         </is>
       </c>
-      <c r="L6" s="2" t="n">
-        <v>45973.95877880897</v>
-      </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -782,9 +762,6 @@
         <is>
           <t>{"enseigne": "E.Leclerc", "magasin": "Espace Technique E.Leclerc", "date": "2025-10-07", "heure": "19:21", "article": "Mario Kart World Switch 2", "prix_unitaire": "69.90", "quantite": "1", "prix_total": "69.90", "total_ticket": "524.85"}</t>
         </is>
-      </c>
-      <c r="L7" s="2" t="n">
-        <v>45973.95877880897</v>
       </c>
     </row>
     <row r="8">
@@ -831,9 +808,6 @@
           <t>{"enseigne": "E.Leclerc", "magasin": "Centre E.Leclerc Viennedis", "date": "2025-10-07", "heure": "20:00", "rayon": "Jardin", "article": "VINAIGRE MEN.SURPUISS 1LT", "prix_unitaire": "1.00", "quantite": "1", "prix_total": "1.00", "remise": "0.00", "prix_final": "1.00", "total_ticket": "161.29"}</t>
         </is>
       </c>
-      <c r="L8" s="2" t="n">
-        <v>45973.95877880897</v>
-      </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -879,9 +853,6 @@
           <t>{"enseigne": "E.Leclerc", "magasin": "Centre E.Leclerc Viennedis", "date": "2025-10-07", "heure": "20:00", "rayon": "Epicerie sal\u00e9e", "article": "LIEBIG VELOUI.LENS POEL.2X30CL", "prix_unitaire": "2.27", "quantite": "1", "prix_total": "2.27", "remise": "0.00", "prix_final": "2.27", "total_ticket": "161.29"}</t>
         </is>
       </c>
-      <c r="L9" s="2" t="n">
-        <v>45973.95877880897</v>
-      </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -927,9 +898,6 @@
           <t>{"enseigne": "E.Leclerc", "magasin": "Centre E.Leclerc Viennedis", "date": "2025-10-07", "heure": "20:00", "rayon": "Surgel\u00e9s", "article": "R. 20 CREPES EMMENTAL", "prix_unitaire": "3.29", "quantite": "1", "prix_total": "3.29", "remise": "0.00", "prix_final": "3.29", "total_ticket": "161.29"}</t>
         </is>
       </c>
-      <c r="L10" s="2" t="n">
-        <v>45973.95877880897</v>
-      </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -975,9 +943,6 @@
           <t>{"enseigne": "E.Leclerc", "magasin": "Centre E.Leclerc Viennedis", "date": "2025-10-07", "heure": "20:00", "rayon": "Surgel\u00e9s", "article": "R TARTE AUX 3 FROMAGES 400G", "prix_unitaire": "2.78", "quantite": "1", "prix_total": "2.78", "remise": "0.00", "prix_final": "2.78", "total_ticket": "161.29"}</t>
         </is>
       </c>
-      <c r="L11" s="2" t="n">
-        <v>45973.95877880897</v>
-      </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -1023,9 +988,6 @@
           <t>{"enseigne": "E.Leclerc", "magasin": "Centre E.Leclerc Viennedis", "date": "2025-10-07", "heure": "20:00", "rayon": "Surgel\u00e9s", "article": "CORDON BLEU HALAL 2KG", "prix_unitaire": "13.99", "quantite": "1", "prix_total": "13.99", "remise": "0.00", "prix_final": "13.99", "total_ticket": "161.29"}</t>
         </is>
       </c>
-      <c r="L12" s="2" t="n">
-        <v>45973.95877880897</v>
-      </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -1071,9 +1033,6 @@
           <t>{"enseigne": "E.Leclerc", "magasin": "Centre E.Leclerc Viennedis", "date": "2025-10-07", "heure": "20:00", "rayon": "Surgel\u00e9s", "article": "TARTE AUX POIREAUX PB 400G", "prix_unitaire": "3.48", "quantite": "1", "prix_total": "3.48", "remise": "0.00", "prix_final": "3.48", "total_ticket": "161.29"}</t>
         </is>
       </c>
-      <c r="L13" s="2" t="n">
-        <v>45973.95877880897</v>
-      </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -1119,9 +1078,6 @@
           <t>{"enseigne": "E.Leclerc", "magasin": "Centre E.Leclerc Viennedis", "date": "2025-10-07", "heure": "20:00", "rayon": "Volaille", "article": "R. YT GRECA STRACCIATEL 4X150G", "prix_unitaire": "2.99", "quantite": "1", "prix_total": "2.99", "remise": "0.00", "prix_final": "2.99", "total_ticket": "161.29"}</t>
         </is>
       </c>
-      <c r="L14" s="2" t="n">
-        <v>45973.95877880897</v>
-      </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -1167,9 +1123,6 @@
           <t>{"enseigne": "E.Leclerc", "magasin": "Centre E.Leclerc Viennedis", "date": "2025-10-07", "heure": "20:00", "rayon": "Volaille", "article": "R. LAIT 1/2ECR ORIY 1L 2x", "prix_unitaire": "1.98", "quantite": "1", "prix_total": "1.98", "remise": "0.00", "prix_final": "1.98", "total_ticket": "161.29"}</t>
         </is>
       </c>
-      <c r="L15" s="2" t="n">
-        <v>45973.95877880897</v>
-      </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -1215,9 +1168,6 @@
           <t>{"enseigne": "E.Leclerc", "magasin": "Centre E.Leclerc Viennedis", "date": "2025-10-07", "heure": "20:00", "rayon": "Volaille", "article": "BEURRE DOUX PRESIDENT 250G", "prix_unitaire": "2.75", "quantite": "1", "prix_total": "2.75", "remise": "0.00", "prix_final": "2.75", "total_ticket": "161.29"}</t>
         </is>
       </c>
-      <c r="L16" s="2" t="n">
-        <v>45973.95877880897</v>
-      </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -1263,9 +1213,6 @@
           <t>{"enseigne": "E.Leclerc", "magasin": "Centre E.Leclerc Viennedis", "date": "2025-10-07", "heure": "20:00", "rayon": "Cr\u00e9merie", "article": "EMMENTAL RAPE PDT 29%MG 200D", "prix_unitaire": "2.04", "quantite": "1", "prix_total": "2.04", "remise": "0.00", "prix_final": "2.04", "total_ticket": "161.29"}</t>
         </is>
       </c>
-      <c r="L17" s="2" t="n">
-        <v>45973.95877880897</v>
-      </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
@@ -1311,9 +1258,6 @@
           <t>{"enseigne": "E.Leclerc", "magasin": "Centre E.Leclerc Viennedis", "date": "2025-10-07", "heure": "20:00", "rayon": "Cr\u00e9merie", "article": "RACLETTE CARACTERE 420G", "prix_unitaire": "6.54", "quantite": "1", "prix_total": "6.54", "remise": "0.00", "prix_final": "6.54", "total_ticket": "161.29"}</t>
         </is>
       </c>
-      <c r="L18" s="2" t="n">
-        <v>45973.95877880897</v>
-      </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
@@ -1359,9 +1303,6 @@
           <t>{"enseigne": "E.Leclerc", "magasin": "Centre E.Leclerc Viennedis", "date": "2025-10-07", "heure": "20:00", "rayon": "Cr\u00e9merie", "article": "RAEL.CLASSIQ.LAIT RMP 420G", "prix_unitaire": "5.35", "quantite": "1", "prix_total": "5.35", "remise": "0.00", "prix_final": "5.35", "total_ticket": "161.29"}</t>
         </is>
       </c>
-      <c r="L19" s="2" t="n">
-        <v>45973.95877880897</v>
-      </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
@@ -1407,9 +1348,6 @@
           <t>{"enseigne": "E.Leclerc", "magasin": "Centre E.Leclerc Viennedis", "date": "2025-10-07", "heure": "20:00", "rayon": "Cr\u00e9merie", "article": "BRIQUE AFFINEE 150G", "prix_unitaire": "2.64", "quantite": "1", "prix_total": "2.64", "remise": "0.00", "prix_final": "2.64", "total_ticket": "161.29"}</t>
         </is>
       </c>
-      <c r="L20" s="2" t="n">
-        <v>45973.95877880897</v>
-      </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
@@ -1455,9 +1393,6 @@
           <t>{"enseigne": "E.Leclerc", "magasin": "Centre E.Leclerc Viennedis", "date": "2025-10-07", "heure": "20:00", "rayon": "Hygi\u00e8ne", "article": "ESSUIE-TOUT BLANC X6", "prix_unitaire": "3.70", "quantite": "1", "prix_total": "3.70", "remise": "0.00", "prix_final": "3.70", "total_ticket": "161.29"}</t>
         </is>
       </c>
-      <c r="L21" s="2" t="n">
-        <v>45973.95877880897</v>
-      </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
@@ -1503,9 +1438,6 @@
           <t>{"enseigne": "E.Leclerc", "magasin": "Centre E.Leclerc Viennedis", "date": "2025-10-07", "heure": "20:00", "rayon": "Droguerie", "article": "GARN MALINI DETERGENT", "prix_unitaire": "16.33", "quantite": "1", "prix_total": "16.33", "remise": "0.00", "prix_final": "16.33", "total_ticket": "161.29"}</t>
         </is>
       </c>
-      <c r="L22" s="2" t="n">
-        <v>45973.95877880897</v>
-      </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
@@ -1551,9 +1483,6 @@
           <t>{"enseigne": "E.Leclerc", "magasin": "Centre E.Leclerc Viennedis", "date": "2025-10-07", "heure": "20:00", "rayon": "Eaux bi\u00e8res", "article": "POMS JUCE CAROTT/CITRON 75CL", "prix_unitaire": "1.68", "quantite": "1", "prix_total": "1.68", "remise": "0.00", "prix_final": "1.68", "total_ticket": "161.29"}</t>
         </is>
       </c>
-      <c r="L23" s="2" t="n">
-        <v>45973.95877880897</v>
-      </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
@@ -1599,9 +1528,6 @@
           <t>{"enseigne": "E.Leclerc", "magasin": "Centre E.Leclerc Viennedis", "date": "2025-10-07", "heure": "20:00", "rayon": "Eaux bi\u00e8res", "article": "COCA-COLA ORIGINAL 6X1.75L", "prix_unitaire": "14.28", "quantite": "1", "prix_total": "14.28", "remise": "0.00", "prix_final": "14.28", "total_ticket": "161.29"}</t>
         </is>
       </c>
-      <c r="L24" s="2" t="n">
-        <v>45973.95877880897</v>
-      </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
@@ -1647,9 +1573,6 @@
           <t>{"enseigne": "E.Leclerc", "magasin": "Centre E.Leclerc Viennedis", "date": "2025-10-07", "heure": "20:00", "rayon": "Eaux bi\u00e8res", "article": "BIERE 1664 BLONDE 18X25CL", "prix_unitaire": "11.76", "quantite": "1", "prix_total": "11.76", "remise": "0.00", "prix_final": "11.76", "total_ticket": "161.29"}</t>
         </is>
       </c>
-      <c r="L25" s="2" t="n">
-        <v>45973.95877880897</v>
-      </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
@@ -1695,9 +1618,6 @@
           <t>{"enseigne": "E.Leclerc", "magasin": "Centre E.Leclerc Viennedis", "date": "2025-10-07", "heure": "20:00", "rayon": "Eaux bi\u00e8res", "article": "BIERE 1664 BLANC 6X25CL", "prix_unitaire": "4.71", "quantite": "1", "prix_total": "4.71", "remise": "0.00", "prix_final": "4.71", "total_ticket": "161.29"}</t>
         </is>
       </c>
-      <c r="L26" s="2" t="n">
-        <v>45973.95877880897</v>
-      </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
@@ -1743,9 +1663,6 @@
           <t>{"enseigne": "E.Leclerc", "magasin": "Centre E.Leclerc Viennedis", "date": "2025-10-07", "heure": "20:00", "rayon": "Vins", "article": "PAYS D'OC O.CANBRAS SBLC5", "prix_unitaire": "14.95", "quantite": "1", "prix_total": "14.95", "remise": "0.00", "prix_final": "14.95", "total_ticket": "161.29"}</t>
         </is>
       </c>
-      <c r="L27" s="2" t="n">
-        <v>45973.95877880897</v>
-      </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
@@ -1791,9 +1708,6 @@
           <t>{"enseigne": "E.Leclerc", "magasin": "Centre E.Leclerc Viennedis", "date": "2025-10-07", "heure": "20:00", "rayon": "Conserves", "article": "ONE CHAT STERIL.BOEUF BLE 3KG", "prix_unitaire": "13.12", "quantite": "1", "prix_total": "13.12", "remise": "0.00", "prix_final": "13.12", "total_ticket": "161.29"}</t>
         </is>
       </c>
-      <c r="L28" s="2" t="n">
-        <v>45973.95877880897</v>
-      </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
@@ -1839,9 +1753,6 @@
           <t>{"enseigne": "E.Leclerc", "magasin": "Centre E.Leclerc Viennedis", "date": "2025-10-07", "heure": "20:00", "rayon": "Conserves", "article": "MS.CASSOULET 1/2", "prix_unitaire": "1.90", "quantite": "1", "prix_total": "1.90", "remise": "0.00", "prix_final": "1.90", "total_ticket": "161.29"}</t>
         </is>
       </c>
-      <c r="L29" s="2" t="n">
-        <v>45973.95877880897</v>
-      </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
@@ -1887,9 +1798,6 @@
           <t>{"enseigne": "E.Leclerc", "magasin": "Centre E.Leclerc Viennedis", "date": "2025-10-07", "heure": "20:00", "rayon": "Conserves", "article": "DAUCY.HARIOUT.GARNIE 1/2", "prix_unitaire": "2.26", "quantite": "1", "prix_total": "2.26", "remise": "0.00", "prix_final": "2.26", "total_ticket": "161.29"}</t>
         </is>
       </c>
-      <c r="L30" s="2" t="n">
-        <v>45973.95877880897</v>
-      </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
@@ -1935,9 +1843,6 @@
           <t>{"enseigne": "E.Leclerc", "magasin": "Centre E.Leclerc Viennedis", "date": "2025-10-07", "heure": "20:00", "rayon": "Epicerie sal\u00e9e", "article": "FREEDENTMIT.MENT.VT.5X10DRA8", "prix_unitaire": "2.15", "quantite": "1", "prix_total": "2.15", "remise": "0.00", "prix_final": "2.15", "total_ticket": "161.29"}</t>
         </is>
       </c>
-      <c r="L31" s="2" t="n">
-        <v>45973.95877880897</v>
-      </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
@@ -1983,9 +1888,6 @@
           <t>{"enseigne": "E.Leclerc", "magasin": "Centre E.Leclerc Viennedis", "date": "2025-10-07", "heure": "20:00", "rayon": "Epicerie sal\u00e9e", "article": "R.BAGUETTES PRE-CUITES 2X150B", "prix_unitaire": "1.36", "quantite": "1", "prix_total": "1.36", "remise": "0.00", "prix_final": "1.36", "total_ticket": "161.29"}</t>
         </is>
       </c>
-      <c r="L32" s="2" t="n">
-        <v>45973.95877880897</v>
-      </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
@@ -2031,9 +1933,6 @@
           <t>{"enseigne": "E.Leclerc", "magasin": "Centre E.Leclerc Viennedis", "date": "2025-10-07", "heure": "20:00", "rayon": "Epicerie sal\u00e9e", "article": "ECOT.COMPOTE POMME 4X100G", "prix_unitaire": "1.65", "quantite": "1", "prix_total": "1.65", "remise": "0.00", "prix_final": "1.65", "total_ticket": "161.29"}</t>
         </is>
       </c>
-      <c r="L33" s="2" t="n">
-        <v>45973.95877880897</v>
-      </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
@@ -2079,9 +1978,6 @@
           <t>{"enseigne": "E.Leclerc", "magasin": "Centre E.Leclerc Viennedis", "date": "2025-10-07", "heure": "20:00", "rayon": "Epicerie sal\u00e9e", "article": "PASA.PRINS AU LAIT X 10", "prix_unitaire": "1.40", "quantite": "1", "prix_total": "1.40", "remise": "0.00", "prix_final": "1.40", "total_ticket": "161.29"}</t>
         </is>
       </c>
-      <c r="L34" s="2" t="n">
-        <v>45973.95877880897</v>
-      </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
@@ -2127,9 +2023,6 @@
           <t>{"enseigne": "E.Leclerc", "magasin": "Centre E.Leclerc Viennedis", "date": "2025-10-07", "heure": "20:00", "rayon": "Epicerie sal\u00e9e", "article": "MAILL.MOUT.MI-FO DCL", "prix_unitaire": "1.92", "quantite": "1", "prix_total": "1.92", "remise": "0.00", "prix_final": "1.92", "total_ticket": "161.29"}</t>
         </is>
       </c>
-      <c r="L35" s="2" t="n">
-        <v>45973.95877880897</v>
-      </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
@@ -2175,9 +2068,6 @@
           <t>{"enseigne": "E.Leclerc", "magasin": "Centre E.Leclerc Viennedis", "date": "2025-10-07", "heure": "20:00", "rayon": "Epicerie sal\u00e9e", "article": "BARILLA PENNE RIGATE 500G", "prix_unitaire": "1.01", "quantite": "1", "prix_total": "1.01", "remise": "0.00", "prix_final": "1.01", "total_ticket": "161.29"}</t>
         </is>
       </c>
-      <c r="L36" s="2" t="n">
-        <v>45973.95877880897</v>
-      </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
@@ -2223,9 +2113,6 @@
           <t>{"enseigne": "E.Leclerc", "magasin": "Centre E.Leclerc Viennedis", "date": "2025-10-07", "heure": "20:00", "rayon": "Epicerie sal\u00e9e", "article": "R.VINAIGRE BALSAM.MODENE", "prix_unitaire": "1.57", "quantite": "1", "prix_total": "1.57", "remise": "0.00", "prix_final": "1.57", "total_ticket": "161.29"}</t>
         </is>
       </c>
-      <c r="L37" s="2" t="n">
-        <v>45973.95877880897</v>
-      </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
@@ -2271,9 +2158,6 @@
           <t>{"enseigne": "E.Leclerc", "magasin": "Centre E.Leclerc Viennedis", "date": "2025-10-07", "heure": "20:00", "rayon": "Epicerie sal\u00e9e", "article": "R.JUS CIT URON.SICILE 2X125ML", "prix_unitaire": "1.06", "quantite": "1", "prix_total": "1.06", "remise": "0.00", "prix_final": "1.06", "total_ticket": "161.29"}</t>
         </is>
       </c>
-      <c r="L38" s="2" t="n">
-        <v>45973.95877880897</v>
-      </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
@@ -2319,9 +2203,6 @@
           <t>{"enseigne": "E.Leclerc", "magasin": "Centre E.Leclerc Viennedis", "date": "2025-10-07", "heure": "20:00", "rayon": "Epicerie sal\u00e9e", "article": "CACAHUETES GRILLEES 450G", "prix_unitaire": "3.49", "quantite": "1", "prix_total": "3.49", "remise": "0.00", "prix_final": "3.49", "total_ticket": "161.29"}</t>
         </is>
       </c>
-      <c r="L39" s="2" t="n">
-        <v>45973.95877880897</v>
-      </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
@@ -2367,9 +2248,6 @@
           <t>{"enseigne": "E.Leclerc", "magasin": "Centre E.Leclerc Viennedis", "date": "2025-10-07", "heure": "20:00", "rayon": "Epicerie sal\u00e9e", "article": "PASA.CROUTONS SOUPE AIL 4x", "prix_unitaire": "3.96", "quantite": "1", "prix_total": "3.96", "remise": "0.00", "prix_final": "3.96", "total_ticket": "161.29"}</t>
         </is>
       </c>
-      <c r="L40" s="2" t="n">
-        <v>45973.95877880897</v>
-      </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
@@ -2415,9 +2293,6 @@
           <t>{"enseigne": "E.Leclerc", "magasin": "Centre E.Leclerc Viennedis", "date": "2025-10-07", "heure": "20:00", "rayon": "Epicerie sal\u00e9e", "article": "NOUL POIV NR GRAIN CLASS", "prix_unitaire": "2.95", "quantite": "1", "prix_total": "2.95", "remise": "0.00", "prix_final": "2.95", "total_ticket": "161.29"}</t>
         </is>
       </c>
-      <c r="L41" s="2" t="n">
-        <v>45973.95877880897</v>
-      </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
@@ -2463,9 +2338,6 @@
           <t>{"enseigne": "E.Leclerc", "magasin": "Centre E.Leclerc Viennedis", "date": "2025-10-07", "heure": "20:00", "rayon": "Epicerie sal\u00e9e", "article": "TENDRE BANSETTES CEL.500G", "prix_unitaire": "1.17", "quantite": "1", "prix_total": "1.17", "remise": "0.00", "prix_final": "1.17", "total_ticket": "161.29"}</t>
         </is>
       </c>
-      <c r="L42" s="2" t="n">
-        <v>45973.95877880897</v>
-      </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
@@ -2511,9 +2383,6 @@
           <t>{"enseigne": "E.Leclerc", "magasin": "Centre E.Leclerc Viennedis", "date": "2025-10-07", "heure": "20:00", "rayon": "Conserves", "article": "SAUP.THON CATALANE 2X1/6", "prix_unitaire": "2.19", "quantite": "1", "prix_total": "2.19", "remise": "0.00", "prix_final": "2.19", "total_ticket": "161.29"}</t>
         </is>
       </c>
-      <c r="L43" s="2" t="n">
-        <v>45973.95877880897</v>
-      </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
@@ -2559,9 +2428,6 @@
           <t>{"enseigne": "Action", "magasin": "4445/ Rillieux-la-Pape", "date": "2025-10-08", "heure": "20:23", "code_article": "2567527", "article": "plaque stationnement plastique noir", "prix_unitaire": "0.57", "quantite": "1", "prix_total": "0.57", "total_ticket": "192.20"}</t>
         </is>
       </c>
-      <c r="L44" s="2" t="n">
-        <v>45973.95877880897</v>
-      </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
@@ -2607,9 +2473,6 @@
           <t>{"enseigne": "Action", "magasin": "4445/ Rillieux-la-Pape", "date": "2025-10-08", "heure": "20:23", "code_article": "3001106", "article": "hotel royal serviette 70x140cm blanc", "prix_unitaire": "5.99", "quantite": "1", "prix_total": "5.99", "total_ticket": "192.20"}</t>
         </is>
       </c>
-      <c r="L45" s="2" t="n">
-        <v>45973.95877880897</v>
-      </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
@@ -2655,9 +2518,6 @@
           <t>{"enseigne": "Action", "magasin": "4445/ Rillieux-la-Pape", "date": "2025-10-08", "heure": "20:23", "code_article": "2576183", "article": "alaskas temp 100gr fruits mer &amp; saumon", "prix_unitaire": "1.88", "quantite": "1", "prix_total": "1.88", "total_ticket": "192.20"}</t>
         </is>
       </c>
-      <c r="L46" s="2" t="n">
-        <v>45973.95877880897</v>
-      </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
@@ -2703,9 +2563,6 @@
           <t>{"enseigne": "Action", "magasin": "4445/ Rillieux-la-Pape", "date": "2025-10-08", "heure": "20:23", "code_article": "3202385", "article": "brinde d'\u00e9tanch\u00e9it\u00e9 20mm trans", "prix_unitaire": "1.49", "quantite": "1", "prix_total": "1.49", "total_ticket": "192.20"}</t>
         </is>
       </c>
-      <c r="L47" s="2" t="n">
-        <v>45973.95877880897</v>
-      </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
@@ -2751,9 +2608,6 @@
           <t>{"enseigne": "Action", "magasin": "4445/ Rillieux-la-Pape", "date": "2025-10-08", "heure": "20:23", "code_article": "3215179", "article": "set torchons de luxe 3pcs 50x70cm", "prix_unitaire": "4.49", "quantite": "1", "prix_total": "4.49", "total_ticket": "192.20"}</t>
         </is>
       </c>
-      <c r="L48" s="2" t="n">
-        <v>45973.95877880897</v>
-      </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
@@ -2799,9 +2653,6 @@
           <t>{"enseigne": "Action", "magasin": "4445/ Rillieux-la-Pape", "date": "2025-10-08", "heure": "20:23", "code_article": "2550245", "article": "dumil papier sulfuris\u00e9 8m", "prix_unitaire": "0.89", "quantite": "1", "prix_total": "0.89", "total_ticket": "192.20"}</t>
         </is>
       </c>
-      <c r="L49" s="2" t="n">
-        <v>45973.95877880897</v>
-      </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
@@ -2847,9 +2698,6 @@
           <t>{"enseigne": "Action", "magasin": "4445/ Rillieux-la-Pape", "date": "2025-10-08", "heure": "20:23", "code_article": "2540899", "article": "studio home miroir porte 34x94cm", "prix_unitaire": "7.95", "quantite": "1", "prix_total": "7.95", "total_ticket": "192.20"}</t>
         </is>
       </c>
-      <c r="L50" s="2" t="n">
-        <v>45973.95877880897</v>
-      </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
@@ -2895,9 +2743,6 @@
           <t>{"enseigne": "Action", "magasin": "4445/ Rillieux-la-Pape", "date": "2025-10-08", "heure": "20:23", "code_article": "3210149", "article": "joe film plastique distr. 50mx10cm 2pcs", "prix_unitaire": "1.99", "quantite": "1", "prix_total": "1.99", "total_ticket": "192.20"}</t>
         </is>
       </c>
-      <c r="L51" s="2" t="n">
-        <v>45973.95877880897</v>
-      </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
@@ -2943,9 +2788,6 @@
           <t>{"enseigne": "Action", "magasin": "4445/ Rillieux-la-Pape", "date": "2025-10-08", "heure": "20:23", "code_article": "3205763", "article": "fentre anti-bu\u00e9e plun protections sol", "prix_unitaire": "0.65", "quantite": "1", "prix_total": "0.65", "total_ticket": "192.20"}</t>
         </is>
       </c>
-      <c r="L52" s="2" t="n">
-        <v>45973.95877880897</v>
-      </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
@@ -2991,9 +2833,6 @@
           <t>{"enseigne": "Action", "magasin": "4445/ Rillieux-la-Pape", "date": "2025-10-08", "heure": "20:23", "code_article": "2511736", "article": "action sac \u00e0 comm. 48x48x17cm bleu/blanc", "prix_unitaire": "1.19", "quantite": "1", "prix_total": "1.19", "total_ticket": "192.20"}</t>
         </is>
       </c>
-      <c r="L53" s="2" t="n">
-        <v>45973.95877880897</v>
-      </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
@@ -3039,9 +2878,6 @@
           <t>{"enseigne": "Action", "magasin": "4445/ Rillieux-la-Pape", "date": "2025-10-08", "heure": "20:23", "code_article": "2576034", "article": "film alimentaire 50ml", "prix_unitaire": "0.80", "quantite": "1", "prix_total": "0.80", "total_ticket": "192.20"}</t>
         </is>
       </c>
-      <c r="L54" s="2" t="n">
-        <v>45973.95877880897</v>
-      </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
@@ -3087,9 +2923,6 @@
           <t>{"enseigne": "Action", "magasin": "4445/ Rillieux-la-Pape", "date": "2025-10-08", "heure": "20:23", "code_article": "292106", "article": "domil film chanois naturelle xl 48x33cm", "prix_unitaire": "3.99", "quantite": "1", "prix_total": "3.99", "total_ticket": "192.20"}</t>
         </is>
       </c>
-      <c r="L55" s="2" t="n">
-        <v>45973.95877880897</v>
-      </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
@@ -3135,9 +2968,6 @@
           <t>{"enseigne": "Action", "magasin": "4445/ Rillieux-la-Pape", "date": "2025-10-08", "heure": "20:23", "code_article": "3206928", "article": "domil film chanois naturelle xl 50m", "prix_unitaire": "3.38", "quantite": "1", "prix_total": "3.38", "total_ticket": "192.20"}</t>
         </is>
       </c>
-      <c r="L56" s="2" t="n">
-        <v>45973.95877880897</v>
-      </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
@@ -3183,9 +3013,6 @@
           <t>{"enseigne": "Action", "magasin": "4445/ Rillieux-la-Pape", "date": "2025-10-08", "heure": "20:23", "code_article": "2557112", "article": "dumil sachets \u00e0 curseur 2pcs 1l", "prix_unitaire": "1.96", "quantite": "1", "prix_total": "1.96", "total_ticket": "192.20"}</t>
         </is>
       </c>
-      <c r="L57" s="2" t="n">
-        <v>45973.95877880897</v>
-      </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
@@ -3231,9 +3058,6 @@
           <t>{"enseigne": "Action", "magasin": "4445/ Rillieux-la-Pape", "date": "2025-10-08", "heure": "20:23", "code_article": "3213117", "article": "ambi pur d\u00e9sodorisant 185ml light citrus", "prix_unitaire": "2.77", "quantite": "1", "prix_total": "2.77", "total_ticket": "192.20"}</t>
         </is>
       </c>
-      <c r="L58" s="2" t="n">
-        <v>45973.95877880897</v>
-      </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
@@ -3279,9 +3103,6 @@
           <t>{"enseigne": "Action", "magasin": "4445/ Rillieux-la-Pape", "date": "2025-10-08", "heure": "20:23", "code_article": "3008099", "article": "microfiber dish blocks 10x10x6.5cm 2pcs", "prix_unitaire": "2.16", "quantite": "1", "prix_total": "2.16", "total_ticket": "192.20"}</t>
         </is>
       </c>
-      <c r="L59" s="2" t="n">
-        <v>45973.95877880897</v>
-      </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
@@ -3327,9 +3148,6 @@
           <t>{"enseigne": "Action", "magasin": "4445/ Rillieux-la-Pape", "date": "2025-10-08", "heure": "20:23", "code_article": "3203286", "article": "server creanisateur rotin plastique 51", "prix_unitaire": "1.64", "quantite": "1", "prix_total": "1.64", "total_ticket": "192.20"}</t>
         </is>
       </c>
-      <c r="L60" s="2" t="n">
-        <v>45973.95877880897</v>
-      </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
@@ -3375,9 +3193,6 @@
           <t>{"enseigne": "Action", "magasin": "4445/ Rillieux-la-Pape", "date": "2025-10-08", "heure": "20:23", "code_article": "2565880", "article": "giada beauty d\u00e9sodorisant fresh berries", "prix_unitaire": "2.33", "quantite": "1", "prix_total": "2.33", "total_ticket": "192.20"}</t>
         </is>
       </c>
-      <c r="L61" s="2" t="n">
-        <v>45973.95877880897</v>
-      </c>
     </row>
     <row r="62">
       <c r="A62" t="n">
@@ -3423,9 +3238,6 @@
           <t>{"enseigne": "Action", "magasin": "4445/ Rillieux-la-Pape", "date": "2025-10-08", "heure": "20:23", "code_article": "3016206", "article": "st tropez deo spray st 95lav. tropical", "prix_unitaire": "5.59", "quantite": "1", "prix_total": "5.59", "total_ticket": "192.20"}</t>
         </is>
       </c>
-      <c r="L62" s="2" t="n">
-        <v>45973.95877880897</v>
-      </c>
     </row>
     <row r="63">
       <c r="A63" t="n">
@@ -3471,9 +3283,6 @@
           <t>{"enseigne": "Action", "magasin": "4445/ Rillieux-la-Pape", "date": "2025-10-08", "heure": "20:23", "code_article": "3218527", "article": "chanteclair d\u00e9graissant 750ml marseille", "prix_unitaire": "2.29", "quantite": "1", "prix_total": "2.29", "total_ticket": "192.20"}</t>
         </is>
       </c>
-      <c r="L63" s="2" t="n">
-        <v>45973.95877880897</v>
-      </c>
     </row>
     <row r="64">
       <c r="A64" t="n">
@@ -3519,9 +3328,6 @@
           <t>{"enseigne": "Action", "magasin": "4445/ Rillieux-la-Pape", "date": "2025-10-08", "heure": "20:23", "code_article": "2546422", "article": "chiffon microfibre 4pcs 32x30cm", "prix_unitaire": "0.99", "quantite": "1", "prix_total": "0.99", "total_ticket": "192.20"}</t>
         </is>
       </c>
-      <c r="L64" s="2" t="n">
-        <v>45973.95877880897</v>
-      </c>
     </row>
     <row r="65">
       <c r="A65" t="n">
@@ -3567,9 +3373,6 @@
           <t>{"enseigne": "Action", "magasin": "4445/ Rillieux-la-Pape", "date": "2025-10-08", "heure": "20:23", "code_article": "2505686", "article": "torche=clou marteau rouge=clou bois", "prix_unitaire": "3.67", "quantite": "1", "prix_total": "3.67", "total_ticket": "192.20"}</t>
         </is>
       </c>
-      <c r="L65" s="2" t="n">
-        <v>45973.95877880897</v>
-      </c>
     </row>
     <row r="66">
       <c r="A66" t="n">
@@ -3615,9 +3418,6 @@
           <t>{"enseigne": "Action", "magasin": "4445/ Rillieux-la-Pape", "date": "2025-10-08", "heure": "20:23", "code_article": "2507070", "article": "rideau en microfibre 54x14cm", "prix_unitaire": "0.92", "quantite": "1", "prix_total": "0.92", "total_ticket": "192.20"}</t>
         </is>
       </c>
-      <c r="L66" s="2" t="n">
-        <v>45973.95877880897</v>
-      </c>
     </row>
     <row r="67">
       <c r="A67" t="n">
@@ -3663,9 +3463,6 @@
           <t>{"enseigne": "Action", "magasin": "4445/ Rillieux-la-Pape", "date": "2025-10-08", "heure": "20:23", "code_article": "3205535", "article": "parfum de luxe homme 150ml white label", "prix_unitaire": "5.98", "quantite": "1", "prix_total": "5.98", "total_ticket": "192.20"}</t>
         </is>
       </c>
-      <c r="L67" s="2" t="n">
-        <v>45973.95877880897</v>
-      </c>
     </row>
     <row r="68">
       <c r="A68" t="n">
@@ -3711,9 +3508,6 @@
           <t>{"enseigne": "Action", "magasin": "4445/ Rillieux-la-Pape", "date": "2025-10-08", "heure": "20:23", "code_article": "3004590", "article": "fashion professional shamp 1l keratine", "prix_unitaire": "2.49", "quantite": "1", "prix_total": "2.49", "total_ticket": "192.20"}</t>
         </is>
       </c>
-      <c r="L68" s="2" t="n">
-        <v>45973.95877880897</v>
-      </c>
     </row>
     <row r="69">
       <c r="A69" t="n">
@@ -3759,9 +3553,6 @@
           <t>{"enseigne": "Action", "magasin": "4445/ Rillieux-la-Pape", "date": "2025-10-08", "heure": "20:23", "code_article": "3000035", "article": "tio think deakwity itch b pots", "prix_unitaire": "9.99", "quantite": "1", "prix_total": "9.99", "total_ticket": "192.20"}</t>
         </is>
       </c>
-      <c r="L69" s="2" t="n">
-        <v>45973.95877880897</v>
-      </c>
     </row>
     <row r="70">
       <c r="A70" t="n">
@@ -3807,9 +3598,6 @@
           <t>{"enseigne": "Action", "magasin": "4445/ Rillieux-la-Pape", "date": "2025-10-08", "heure": "20:23", "code_article": "1321418", "article": "protextreme gel coiffure 750ml sweet honey", "prix_unitaire": "2.44", "quantite": "1", "prix_total": "2.44", "total_ticket": "192.20"}</t>
         </is>
       </c>
-      <c r="L70" s="2" t="n">
-        <v>45973.95877880897</v>
-      </c>
     </row>
     <row r="71">
       <c r="A71" t="n">
@@ -3855,9 +3643,6 @@
           <t>{"enseigne": "Action", "magasin": "4445/ Rillieux-la-Pape", "date": "2025-10-08", "heure": "20:23", "code_article": "3217153", "article": "rideau occultant shiny noir260cm", "prix_unitaire": "12.95", "quantite": "1", "prix_total": "12.95", "total_ticket": "192.20"}</t>
         </is>
       </c>
-      <c r="L71" s="2" t="n">
-        <v>45973.95877880897</v>
-      </c>
     </row>
     <row r="72">
       <c r="A72" t="n">
@@ -3903,9 +3688,6 @@
           <t>{"enseigne": "Action", "magasin": "4445/ Rillieux-la-Pape", "date": "2025-10-08", "heure": "20:23", "code_article": "2531240", "article": "chaussettes sport lotto noir/3pr 39-46", "prix_unitaire": "2.99", "quantite": "1", "prix_total": "2.99", "total_ticket": "192.20"}</t>
         </is>
       </c>
-      <c r="L72" s="2" t="n">
-        <v>45973.95877880897</v>
-      </c>
     </row>
     <row r="73">
       <c r="A73" t="n">
@@ -3951,9 +3733,6 @@
           <t>{"enseigne": "Action", "magasin": "4445/ Rillieux-la-Pape", "date": "2025-10-08", "heure": "20:23", "code_article": "2507308", "article": "audidas deo spray 150ml dynamic pulse", "prix_unitaire": "2.19", "quantite": "1", "prix_total": "2.19", "total_ticket": "192.20"}</t>
         </is>
       </c>
-      <c r="L73" s="2" t="n">
-        <v>45973.95877880897</v>
-      </c>
     </row>
     <row r="74">
       <c r="A74" t="n">
@@ -3999,9 +3778,6 @@
           <t>{"enseigne": "Action", "magasin": "4445/ Rillieux-la-Pape", "date": "2025-10-08", "heure": "20:23", "code_article": "2561275", "article": "bord go tni150 aff 30x40cm", "prix_unitaire": "1.79", "quantite": "1", "prix_total": "1.79", "total_ticket": "192.20"}</t>
         </is>
       </c>
-      <c r="L74" s="2" t="n">
-        <v>45973.95877880897</v>
-      </c>
     </row>
     <row r="75">
       <c r="A75" t="n">
@@ -4047,9 +3823,6 @@
           <t>{"enseigne": "Action", "magasin": "4445/ Rillieux-la-Pape", "date": "2025-10-08", "heure": "20:23", "code_article": "3211675", "article": "bougie parfum\u00e9e art 10x12.5cm div.cl.", "prix_unitaire": "4.79", "quantite": "1", "prix_total": "4.79", "total_ticket": "192.20"}</t>
         </is>
       </c>
-      <c r="L75" s="2" t="n">
-        <v>45973.95877880897</v>
-      </c>
     </row>
     <row r="76">
       <c r="A76" t="n">
@@ -4095,9 +3868,6 @@
           <t>{"enseigne": "Action", "magasin": "4445/ Rillieux-la-Pape", "date": "2025-10-08", "heure": "20:23", "code_article": "2527703", "article": "max en microwaves feuilles jusqu'\u00e0 2m", "prix_unitaire": "2.59", "quantite": "1", "prix_total": "2.59", "total_ticket": "192.20"}</t>
         </is>
       </c>
-      <c r="L76" s="2" t="n">
-        <v>45973.95877880897</v>
-      </c>
     </row>
     <row r="77">
       <c r="A77" t="n">
@@ -4143,9 +3913,6 @@
           <t>{"enseigne": "Action", "magasin": "4445/ Rillieux-la-Pape", "date": "2025-10-08", "heure": "20:23", "code_article": "2506544", "article": "epargo linquettes menage lumineu", "prix_unitaire": "3.96", "quantite": "1", "prix_total": "3.96", "total_ticket": "192.20"}</t>
         </is>
       </c>
-      <c r="L77" s="2" t="n">
-        <v>45973.95877880897</v>
-      </c>
     </row>
     <row r="78">
       <c r="A78" t="n">
@@ -4191,9 +3958,6 @@
           <t>{"enseigne": "Action", "magasin": "4445/ Rillieux-la-Pape", "date": "2025-10-08", "heure": "20:23", "code_article": "3207306", "article": "james so l'homne sport multi+blanc 137cm", "prix_unitaire": "19.99", "quantite": "1", "prix_total": "19.99", "total_ticket": "192.20"}</t>
         </is>
       </c>
-      <c r="L78" s="2" t="n">
-        <v>45973.95877880897</v>
-      </c>
     </row>
     <row r="79">
       <c r="A79" t="n">
@@ -4239,9 +4003,6 @@
           <t>{"enseigne": "McDonald's", "magasin": "Restaurant McDonald's Vienne DT38", "date": "2025-10-12", "heure": "23:09:38", "article": "BOFrites Db1Ched", "quantite": "1", "prix_unitaire": "1.50", "prix_total": "1.50", "composition": "", "type": "supplement", "total_ticket": "12.50", "tva_taux": "10.00", "tva_montant": "1.14"}</t>
         </is>
       </c>
-      <c r="L79" s="2" t="n">
-        <v>45973.95877880897</v>
-      </c>
     </row>
     <row r="80">
       <c r="A80" t="n">
@@ -4287,9 +4048,6 @@
           <t>{"enseigne": "McDonald's", "magasin": "Restaurant McDonald's Vienne DT38", "date": "2025-10-12", "heure": "23:09:38", "article": "Menu McSmart+", "quantite": "1", "prix_unitaire": "6.00", "prix_total": "6.00", "composition": "\\\"Mn McFish Mayo x2|Coke Best Of\\\"", "type": "menu", "total_ticket": "12.50", "tva_taux": "10.00", "tva_montant": "1.14"}</t>
         </is>
       </c>
-      <c r="L80" s="2" t="n">
-        <v>45973.95877880897</v>
-      </c>
     </row>
     <row r="81">
       <c r="A81" t="n">
@@ -4335,9 +4093,6 @@
           <t>{"enseigne": "McDonald's", "magasin": "Restaurant McDonald's Vienne DT38", "date": "2025-10-12", "heure": "23:09:38", "article": "Menu McSmart", "quantite": "1", "prix_unitaire": "5.00", "prix_total": "5.00", "composition": "\\\"Petit Coke:Menu|Frite Pt ds Menu|Mn Ptit Chicken|Mn McFish Mayo\\\"", "type": "menu", "total_ticket": "12.50", "tva_taux": "10.00", "tva_montant": "1.14"}</t>
         </is>
       </c>
-      <c r="L81" s="2" t="n">
-        <v>45973.95877880897</v>
-      </c>
     </row>
     <row r="82">
       <c r="A82" t="n">
@@ -4383,9 +4138,6 @@
           <t>{"enseigne": "Carrefour Market", "magasin": "Market RILLIEUX VILLAGE", "date": "2025-10-14", "heure": "19:36:51", "rayon": "ALIMENTAIRE", "article": "NOUGAT 3 FRUITS", "quantite": "1", "unite": "unit\u00e9", "prix_unitaire": "2.49", "prix_total": "2.49", "remise": "0.00", "prix_final": "2.49", "total_ticket": "76.57"}</t>
         </is>
       </c>
-      <c r="L82" s="2" t="n">
-        <v>45973.95877880897</v>
-      </c>
     </row>
     <row r="83">
       <c r="A83" t="n">
@@ -4431,9 +4183,6 @@
           <t>{"enseigne": "Carrefour Market", "magasin": "Market RILLIEUX VILLAGE", "date": "2025-10-14", "heure": "19:36:51", "rayon": "ALIMENTAIRE", "article": "FIGUE BARNAGTE", "quantite": "0.5984", "unite": "kg", "prix_unitaire": "3.75", "prix_total": "2.23", "remise": "0.00", "prix_final": "2.23", "total_ticket": "76.57"}</t>
         </is>
       </c>
-      <c r="L83" s="2" t="n">
-        <v>45973.95877880897</v>
-      </c>
     </row>
     <row r="84">
       <c r="A84" t="n">
@@ -4479,9 +4228,6 @@
           <t>{"enseigne": "Carrefour Market", "magasin": "Market RILLIEUX VILLAGE", "date": "2025-10-14", "heure": "19:36:51", "rayon": "NON ALIMENTAIRE", "article": "MANCHE TELESCOPIO", "quantite": "1", "unite": "unit\u00e9", "prix_unitaire": "6.40", "prix_total": "6.40", "remise": "0.00", "prix_final": "6.40", "total_ticket": "76.57"}</t>
         </is>
       </c>
-      <c r="L84" s="2" t="n">
-        <v>45973.95877880897</v>
-      </c>
     </row>
     <row r="85">
       <c r="A85" t="n">
@@ -4527,9 +4273,6 @@
           <t>{"enseigne": "Carrefour Market", "magasin": "Market RILLIEUX VILLAGE", "date": "2025-10-14", "heure": "19:36:51", "rayon": "NON ALIMENTAIRE", "article": "50 SACS CONGEL 1L", "quantite": "2", "unite": "unit\u00e9", "prix_unitaire": "1.45", "prix_total": "2.90", "remise": "0.00", "prix_final": "2.90", "total_ticket": "76.57"}</t>
         </is>
       </c>
-      <c r="L85" s="2" t="n">
-        <v>45973.95877880897</v>
-      </c>
     </row>
     <row r="86">
       <c r="A86" t="n">
@@ -4575,9 +4318,6 @@
           <t>{"enseigne": "Carrefour Market", "magasin": "Market RILLIEUX VILLAGE", "date": "2025-10-14", "heure": "19:36:51", "rayon": "NON ALIMENTAIRE", "article": "15 SACS 30L 10gAR", "quantite": "2", "unite": "unit\u00e9", "prix_unitaire": "3.25", "prix_total": "6.50", "remise": "0.00", "prix_final": "6.50", "total_ticket": "76.57"}</t>
         </is>
       </c>
-      <c r="L86" s="2" t="n">
-        <v>45973.95877880897</v>
-      </c>
     </row>
     <row r="87">
       <c r="A87" t="n">
@@ -4623,9 +4363,6 @@
           <t>{"enseigne": "Carrefour Market", "magasin": "Market RILLIEUX VILLAGE", "date": "2025-10-14", "heure": "19:36:51", "rayon": "BEAUTE/SANTE/HYGIENE", "article": "X24 PH 2 PLTS BLAN", "quantite": "1", "unite": "unit\u00e9", "prix_unitaire": "4.69", "prix_total": "4.69", "remise": "-3.86", "prix_final": "0.83", "total_ticket": "76.57"}</t>
         </is>
       </c>
-      <c r="L87" s="2" t="n">
-        <v>45973.95877880897</v>
-      </c>
     </row>
     <row r="88">
       <c r="A88" t="n">
@@ -4671,9 +4408,6 @@
           <t>{"enseigne": "Carrefour Market", "magasin": "Market RILLIEUX VILLAGE", "date": "2025-10-14", "heure": "19:36:51", "rayon": "BEAUTE/SANTE/HYGIENE", "article": "H&amp;S BASE INT CITR", "quantite": "2", "unite": "unit\u00e9", "prix_unitaire": "4.83", "prix_total": "9.66", "remise": "0.00", "prix_final": "9.66", "total_ticket": "76.57"}</t>
         </is>
       </c>
-      <c r="L88" s="2" t="n">
-        <v>45973.95877880897</v>
-      </c>
     </row>
     <row r="89">
       <c r="A89" t="n">
@@ -4719,9 +4453,6 @@
           <t>{"enseigne": "Carrefour Market", "magasin": "Market RILLIEUX VILLAGE", "date": "2025-10-14", "heure": "19:36:51", "rayon": "BEAUTE/SANTE/HYGIENE", "article": "JOUVL DEO IN PU RE", "quantite": "1", "unite": "unit\u00e9", "prix_unitaire": "3.29", "prix_total": "3.29", "remise": "0.00", "prix_final": "3.29", "total_ticket": "76.57"}</t>
         </is>
       </c>
-      <c r="L89" s="2" t="n">
-        <v>45973.95877880897</v>
-      </c>
     </row>
     <row r="90">
       <c r="A90" t="n">
@@ -4767,9 +4498,6 @@
           <t>{"enseigne": "Carrefour Market", "magasin": "Market RILLIEUX VILLAGE", "date": "2025-10-14", "heure": "19:36:51", "rayon": "ALIMENTAIRE", "article": "RAISIN BLANC 500g", "quantite": "1", "unite": "unit\u00e9", "prix_unitaire": "3.99", "prix_total": "3.99", "remise": "0.00", "prix_final": "3.99", "total_ticket": "76.57"}</t>
         </is>
       </c>
-      <c r="L90" s="2" t="n">
-        <v>45973.95877880897</v>
-      </c>
     </row>
     <row r="91">
       <c r="A91" t="n">
@@ -4815,9 +4543,6 @@
           <t>{"enseigne": "Carrefour Market", "magasin": "Market RILLIEUX VILLAGE", "date": "2025-10-14", "heure": "19:36:51", "rayon": "ALIMENTAIRE", "article": "PRUNE JAUNE FR", "quantite": "2", "unite": "unit\u00e9", "prix_unitaire": "1.29", "prix_total": "2.58", "remise": "0.00", "prix_final": "2.58", "total_ticket": "76.57"}</t>
         </is>
       </c>
-      <c r="L91" s="2" t="n">
-        <v>45973.95877880897</v>
-      </c>
     </row>
     <row r="92">
       <c r="A92" t="n">
@@ -4863,9 +4588,6 @@
           <t>{"enseigne": "Carrefour Market", "magasin": "Market RILLIEUX VILLAGE", "date": "2025-10-14", "heure": "19:36:51", "rayon": "ALIMENTAIRE", "article": "PIMENT VERT", "quantite": "0.0898", "unite": "kg", "prix_unitaire": "4.79", "prix_total": "0.43", "remise": "0.00", "prix_final": "0.43", "total_ticket": "76.57"}</t>
         </is>
       </c>
-      <c r="L92" s="2" t="n">
-        <v>45973.95877880897</v>
-      </c>
     </row>
     <row r="93">
       <c r="A93" t="n">
@@ -4911,9 +4633,6 @@
           <t>{"enseigne": "Carrefour Market", "magasin": "Market RILLIEUX VILLAGE", "date": "2025-10-14", "heure": "19:36:51", "rayon": "ALIMENTAIRE", "article": "OIGNON ROUGE 500g", "quantite": "2", "unite": "unit\u00e9", "prix_unitaire": "0.99", "prix_total": "1.98", "remise": "0.00", "prix_final": "1.98", "total_ticket": "76.57"}</t>
         </is>
       </c>
-      <c r="L93" s="2" t="n">
-        <v>45973.95877880897</v>
-      </c>
     </row>
     <row r="94">
       <c r="A94" t="n">
@@ -4959,9 +4678,6 @@
           <t>{"enseigne": "Carrefour Market", "magasin": "Market RILLIEUX VILLAGE", "date": "2025-10-14", "heure": "19:36:51", "rayon": "ALIMENTAIRE", "article": "FLT 1 KG POT SIMP", "quantite": "1", "unite": "unit\u00e9", "prix_unitaire": "0.99", "prix_total": "0.99", "remise": "0.00", "prix_final": "0.99", "total_ticket": "76.57"}</t>
         </is>
       </c>
-      <c r="L94" s="2" t="n">
-        <v>45973.95877880897</v>
-      </c>
     </row>
     <row r="95">
       <c r="A95" t="n">
@@ -5007,9 +4723,6 @@
           <t>{"enseigne": "Carrefour Market", "magasin": "Market RILLIEUX VILLAGE", "date": "2025-10-14", "heure": "19:36:51", "rayon": "ALIMENTAIRE", "article": "FIGUE VIOLET RGF", "quantite": "1", "unite": "unit\u00e9", "prix_unitaire": "5.99", "prix_total": "5.99", "remise": "0.00", "prix_final": "5.99", "total_ticket": "76.57"}</t>
         </is>
       </c>
-      <c r="L95" s="2" t="n">
-        <v>45973.95877880897</v>
-      </c>
     </row>
     <row r="96">
       <c r="A96" t="n">
@@ -5055,9 +4768,6 @@
           <t>{"enseigne": "Carrefour Market", "magasin": "Market RILLIEUX VILLAGE", "date": "2025-10-14", "heure": "19:36:51", "rayon": "ALIMENTAIRE", "article": "DOERADO GRISE", "quantite": "0.4303", "unite": "kg", "prix_unitaire": "15.50", "prix_total": "6.67", "remise": "0.00", "prix_final": "6.67", "total_ticket": "76.57"}</t>
         </is>
       </c>
-      <c r="L96" s="2" t="n">
-        <v>45973.95877880897</v>
-      </c>
     </row>
     <row r="97">
       <c r="A97" t="n">
@@ -5102,9 +4812,6 @@
         <is>
           <t>{"enseigne": "Carrefour Market", "magasin": "Market RILLIEUX VILLAGE", "date": "2025-10-14", "heure": "19:36:51", "rayon": "ALIMENTAIRE", "article": "2XL ALUALLE GAZPA", "quantite": "2", "unite": "unit\u00e9", "prix_unitaire": "6.89", "prix_total": "13.78", "remise": "0.00", "prix_final": "13.78", "total_ticket": "76.57"}</t>
         </is>
-      </c>
-      <c r="L97" s="2" t="n">
-        <v>45973.95877880897</v>
       </c>
     </row>
   </sheetData>

</xml_diff>